<commit_message>
adding the up to date USD correlations
</commit_message>
<xml_diff>
--- a/USD_correlations_rolling_30day_returns.xlsx
+++ b/USD_correlations_rolling_30day_returns.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/02991a894e6c3e62/Desktop/FinTechClassRepo/Class Work/Personal Projects/Macro-Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="25" documentId="114_{F82EAFC5-0B55-4A24-874C-BF173C5F659E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{6724C89B-3948-4F01-AEDB-94960E52F625}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_E0EE6175AE892C02757C4F2559A8408BF031273F" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{FE135FFB-AC4A-4046-9AB8-F32E5A17D0AE}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="33720" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Historical" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="10">
   <si>
     <t>Invesco DB Commodity Index Tracking Fund (DBC)</t>
   </si>
@@ -52,15 +52,6 @@
   </si>
   <si>
     <t>UUP</t>
-  </si>
-  <si>
-    <t>Cross Asset Correlation of Rolling 30 day returns (HISTORICAL)</t>
-  </si>
-  <si>
-    <t>(LAST 15 DAYS)</t>
-  </si>
-  <si>
-    <t>(LAST 30 DAYS)</t>
   </si>
 </sst>
 </file>
@@ -92,7 +83,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -115,175 +106,15 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -622,211 +453,141 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H7"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="43.1796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6328125" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.36328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="7"/>
-      <c r="B1" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="10"/>
-      <c r="B2" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="12" t="s">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2">
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
         <v>0.96</v>
       </c>
-      <c r="D3" s="2">
-        <v>-0.04</v>
-      </c>
-      <c r="E3" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="F3" s="13">
-        <v>-0.37</v>
-      </c>
-      <c r="G3" s="6">
-        <v>-0.56999999999999995</v>
-      </c>
-      <c r="H3" s="2">
-        <v>-0.49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="12" t="s">
+      <c r="D2">
+        <v>0.04</v>
+      </c>
+      <c r="E2">
+        <v>0.71</v>
+      </c>
+      <c r="F2">
+        <v>-0.42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B3">
         <v>0.96</v>
       </c>
-      <c r="C4" s="2">
-        <v>1</v>
-      </c>
-      <c r="D4" s="2">
-        <v>-0.15</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.65</v>
-      </c>
-      <c r="F4" s="13">
-        <v>-0.35</v>
-      </c>
-      <c r="G4" s="6">
-        <v>-0.19</v>
-      </c>
-      <c r="H4" s="2">
-        <v>-0.34</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="12" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>-0.09</v>
+      </c>
+      <c r="E3">
+        <v>0.66</v>
+      </c>
+      <c r="F3">
+        <v>-0.36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="2">
-        <v>-0.04</v>
-      </c>
-      <c r="C5" s="2">
-        <v>-0.15</v>
-      </c>
-      <c r="D5" s="2">
-        <v>1</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="F5" s="13">
+      <c r="B4">
+        <v>0.04</v>
+      </c>
+      <c r="C4">
+        <v>-0.09</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>0.17</v>
+      </c>
+      <c r="F4">
+        <v>-0.45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5">
+        <v>0.71</v>
+      </c>
+      <c r="C5">
+        <v>0.66</v>
+      </c>
+      <c r="D5">
+        <v>0.17</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
         <v>-0.36</v>
       </c>
-      <c r="G5" s="6">
-        <v>-0.83</v>
-      </c>
-      <c r="H5" s="2">
-        <v>-0.31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="2">
-        <v>0.7</v>
-      </c>
-      <c r="C6" s="2">
-        <v>0.65</v>
-      </c>
-      <c r="D6" s="2">
-        <v>0.12</v>
-      </c>
-      <c r="E6" s="2">
-        <v>1</v>
-      </c>
-      <c r="F6" s="13">
-        <v>-0.32</v>
-      </c>
-      <c r="G6" s="6">
-        <v>-0.59</v>
-      </c>
-      <c r="H6" s="2">
-        <v>-0.56999999999999995</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="14" t="s">
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="15">
-        <v>-0.37</v>
-      </c>
-      <c r="C7" s="15">
-        <v>-0.35</v>
-      </c>
-      <c r="D7" s="15">
+      <c r="B6">
+        <v>-0.42</v>
+      </c>
+      <c r="C6">
         <v>-0.36</v>
       </c>
-      <c r="E7" s="15">
-        <v>-0.32</v>
-      </c>
-      <c r="F7" s="16">
-        <v>1</v>
-      </c>
-      <c r="G7" s="6">
-        <v>1</v>
-      </c>
-      <c r="H7" s="2">
+      <c r="D6">
+        <v>-0.45</v>
+      </c>
+      <c r="E6">
+        <v>-0.36</v>
+      </c>
+      <c r="F6">
         <v>1</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:F1"/>
-  </mergeCells>
-  <conditionalFormatting sqref="B3:H7">
-    <cfRule type="colorScale" priority="1">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -835,10 +596,18 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
+      <selection sqref="A1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="4.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.7265625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.08984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
@@ -865,16 +634,16 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.89</v>
+        <v>0.99</v>
       </c>
       <c r="D2">
-        <v>0.27</v>
+        <v>0.97</v>
       </c>
       <c r="E2">
         <v>0.86</v>
       </c>
       <c r="F2">
-        <v>-0.56999999999999995</v>
+        <v>-0.98</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -882,19 +651,19 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>0.89</v>
+        <v>0.99</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>-0.09</v>
+        <v>0.95</v>
       </c>
       <c r="E3">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="F3">
-        <v>-0.19</v>
+        <v>-0.97</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -902,19 +671,19 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>0.27</v>
+        <v>0.97</v>
       </c>
       <c r="C4">
-        <v>-0.09</v>
+        <v>0.95</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>0.28999999999999998</v>
+        <v>0.79</v>
       </c>
       <c r="F4">
-        <v>-0.83</v>
+        <v>-0.98</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -925,16 +694,16 @@
         <v>0.86</v>
       </c>
       <c r="C5">
-        <v>0.7</v>
+        <v>0.85</v>
       </c>
       <c r="D5">
-        <v>0.28999999999999998</v>
+        <v>0.79</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>-0.59</v>
+        <v>-0.82</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -942,16 +711,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>-0.56999999999999995</v>
+        <v>-0.98</v>
       </c>
       <c r="C6">
-        <v>-0.19</v>
+        <v>-0.97</v>
       </c>
       <c r="D6">
-        <v>-0.83</v>
+        <v>-0.98</v>
       </c>
       <c r="E6">
-        <v>-0.59</v>
+        <v>-0.82</v>
       </c>
       <c r="F6">
         <v>1</v>
@@ -966,9 +735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:F1048576"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
@@ -997,16 +764,16 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>0.93</v>
+        <v>0.98</v>
       </c>
       <c r="D2">
-        <v>-0.47</v>
+        <v>0.82</v>
       </c>
       <c r="E2">
-        <v>0.83</v>
+        <v>0.74</v>
       </c>
       <c r="F2">
-        <v>-0.49</v>
+        <v>-0.93</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.35">
@@ -1014,19 +781,19 @@
         <v>6</v>
       </c>
       <c r="B3">
-        <v>0.93</v>
+        <v>0.98</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>-0.63</v>
+        <v>0.77</v>
       </c>
       <c r="E3">
-        <v>0.76</v>
+        <v>0.72</v>
       </c>
       <c r="F3">
-        <v>-0.34</v>
+        <v>-0.93</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.35">
@@ -1034,19 +801,19 @@
         <v>7</v>
       </c>
       <c r="B4">
-        <v>-0.47</v>
+        <v>0.82</v>
       </c>
       <c r="C4">
-        <v>-0.63</v>
+        <v>0.77</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4">
-        <v>-0.38</v>
+        <v>0.36</v>
       </c>
       <c r="F4">
-        <v>-0.31</v>
+        <v>-0.87</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.35">
@@ -1054,19 +821,19 @@
         <v>8</v>
       </c>
       <c r="B5">
-        <v>0.83</v>
+        <v>0.74</v>
       </c>
       <c r="C5">
-        <v>0.76</v>
+        <v>0.72</v>
       </c>
       <c r="D5">
-        <v>-0.38</v>
+        <v>0.36</v>
       </c>
       <c r="E5">
         <v>1</v>
       </c>
       <c r="F5">
-        <v>-0.56999999999999995</v>
+        <v>-0.54</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.35">
@@ -1074,16 +841,16 @@
         <v>9</v>
       </c>
       <c r="B6">
-        <v>-0.49</v>
+        <v>-0.93</v>
       </c>
       <c r="C6">
-        <v>-0.34</v>
+        <v>-0.93</v>
       </c>
       <c r="D6">
-        <v>-0.31</v>
+        <v>-0.87</v>
       </c>
       <c r="E6">
-        <v>-0.56999999999999995</v>
+        <v>-0.54</v>
       </c>
       <c r="F6">
         <v>1</v>

</xml_diff>